<commit_message>
Add pickle load functionality
</commit_message>
<xml_diff>
--- a/Doc/Check_List.xlsx
+++ b/Doc/Check_List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
   <si>
     <t xml:space="preserve">GROUP NAME</t>
   </si>
@@ -281,24 +281,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -553,395 +557,419 @@
   </sheetPr>
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="46.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.22"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="0" t="n">
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="n">
         <v>272</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="0" t="n">
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="n">
         <v>213</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>425</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="0" t="n">
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="n">
         <v>327</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>41</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="0" t="n">
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1" t="n">
         <v>72</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>478</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="0" t="n">
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1" t="n">
         <v>249</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>44</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>440</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>237</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>423</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <v>216</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="0" t="n">
+      <c r="C19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="1" t="n">
         <v>54</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="0" t="n">
+      <c r="C21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="1" t="n">
         <v>98</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="0" t="n">
+      <c r="C24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="1" t="n">
         <v>223</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="0" t="n">
+      <c r="C25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1" t="n">
         <v>219</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="0" t="n">
+      <c r="C26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="1" t="n">
         <v>251</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="0" t="n">
+      <c r="C29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="1" t="n">
         <v>282</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="C31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>484</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="C32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>219</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="C33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>313</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="C41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <v>378</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="0" t="s">
+      <c r="B49" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="0" t="s">
+      <c r="B50" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="0" t="s">
+      <c r="B52" s="1" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added unique value combinations/permutations
</commit_message>
<xml_diff>
--- a/Doc/Check_List.xlsx
+++ b/Doc/Check_List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="57">
   <si>
     <t xml:space="preserve">GROUP NAME</t>
   </si>
@@ -233,7 +233,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -244,6 +244,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.15"/>
         <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -281,7 +287,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -296,6 +302,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -557,8 +567,8 @@
   </sheetPr>
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -780,7 +790,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -790,10 +800,10 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="1" t="n">
@@ -942,29 +952,44 @@
       <c r="B42" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="C42" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="C43" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="C44" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="C45" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="C46" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="4" t="s">
         <v>52</v>
       </c>
     </row>
@@ -977,15 +1002,24 @@
       <c r="B50" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="C50" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="C51" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="1" t="s">
         <v>56</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>